<commit_message>
Extending Documentation - Costs Section
</commit_message>
<xml_diff>
--- a/dokumentation/costs-aws-virtualdesktop.xlsx
+++ b/dokumentation/costs-aws-virtualdesktop.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Dropbox\Studium\Master\IV Semester\CloudComputing\VirtualDesktop-Master\dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C035F3-833B-48CF-B46C-C4A47804D5E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3531F940-C245-453E-A1F6-7C29DF48EF11}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204" xr2:uid="{6BB69F5D-5E78-4C76-8896-0945FFA67CA2}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>10 pro Minute</t>
   </si>
@@ -61,25 +61,13 @@
   <si>
     <t>Lambda</t>
   </si>
-  <si>
-    <t>Summe</t>
-  </si>
-  <si>
-    <t>Mittelwert</t>
-  </si>
-  <si>
-    <t>Laufende Summe</t>
-  </si>
-  <si>
-    <t>Anzahl</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="[$$-409]#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -126,8 +114,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -190,50 +178,11 @@
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
-    <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
-      <c:depthPercent val="100"/>
-      <c:rAngAx val="1"/>
-    </c:view3D>
-    <c:floor>
-      <c:thickness val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
-      </c:spPr>
-    </c:floor>
-    <c:sideWall>
-      <c:thickness val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
-      </c:spPr>
-    </c:sideWall>
-    <c:backWall>
-      <c:thickness val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
-      </c:spPr>
-    </c:backWall>
     <c:plotArea>
       <c:layout/>
-      <c:bar3DChart>
+      <c:barChart>
         <c:barDir val="col"/>
-        <c:grouping val="stacked"/>
+        <c:grouping val="percentStacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -257,7 +206,6 @@
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -297,7 +245,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-798A-4B19-A131-D6E58B9D8511}"/>
+              <c16:uniqueId val="{00000000-74A0-4B3B-A85B-3327C8E793C9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -323,7 +271,6 @@
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -350,10 +297,10 @@
                 <c:formatCode>[$$-409]#,##0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3.43</c:v>
+                  <c:v>3.34</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>350.48</c:v>
+                  <c:v>344.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>230416764.75999999</c:v>
@@ -363,7 +310,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-798A-4B19-A131-D6E58B9D8511}"/>
+              <c16:uniqueId val="{00000001-74A0-4B3B-A85B-3327C8E793C9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -389,7 +336,6 @@
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -429,7 +375,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-798A-4B19-A131-D6E58B9D8511}"/>
+              <c16:uniqueId val="{00000002-74A0-4B3B-A85B-3327C8E793C9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -455,7 +401,6 @@
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -495,7 +440,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-798A-4B19-A131-D6E58B9D8511}"/>
+              <c16:uniqueId val="{00000003-74A0-4B3B-A85B-3327C8E793C9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -521,7 +466,6 @@
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -561,7 +505,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-798A-4B19-A131-D6E58B9D8511}"/>
+              <c16:uniqueId val="{00000004-74A0-4B3B-A85B-3327C8E793C9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -587,7 +531,6 @@
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -614,20 +557,20 @@
                 <c:formatCode>[$$-409]#,##0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>119.07</c:v>
+                  <c:v>131.49</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8008.11</c:v>
+                  <c:v>11053.11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5123906.1100000003</c:v>
+                  <c:v>7366451.1100000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-798A-4B19-A131-D6E58B9D8511}"/>
+              <c16:uniqueId val="{00000005-74A0-4B3B-A85B-3327C8E793C9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -655,7 +598,6 @@
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -695,7 +637,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-798A-4B19-A131-D6E58B9D8511}"/>
+              <c16:uniqueId val="{00000006-74A0-4B3B-A85B-3327C8E793C9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -708,13 +650,12 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:shape val="box"/>
-        <c:axId val="1031166384"/>
-        <c:axId val="1031169664"/>
-        <c:axId val="0"/>
-      </c:bar3DChart>
+        <c:overlap val="100"/>
+        <c:axId val="443142704"/>
+        <c:axId val="443143688"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="1031166384"/>
+        <c:axId val="443142704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -751,7 +692,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1031169664"/>
+        <c:crossAx val="443143688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -759,7 +700,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1031169664"/>
+        <c:axId val="443143688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -779,7 +720,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="[$$-409]#,##0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -810,7 +751,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1031166384"/>
+        <c:crossAx val="443142704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1435,23 +1376,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>922020</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>769620</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Diagramm 5">
+        <xdr:cNvPr id="2" name="Diagramm 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9EF7FCB-9841-4A2C-9A55-A75FEB00CC5A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F957D65-E929-41BD-AAE0-98CE6074DFD1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1772,7 +1713,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1813,10 +1754,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="2">
-        <v>3.43</v>
+        <v>3.34</v>
       </c>
       <c r="C3" s="2">
-        <v>350.48</v>
+        <v>344.2</v>
       </c>
       <c r="D3" s="2">
         <v>230416764.75999999</v>
@@ -1869,13 +1810,13 @@
         <v>8</v>
       </c>
       <c r="B7" s="2">
-        <v>119.07</v>
+        <v>131.49</v>
       </c>
       <c r="C7" s="2">
-        <v>8008.11</v>
+        <v>11053.11</v>
       </c>
       <c r="D7" s="2">
-        <v>5123906.1100000003</v>
+        <v>7366451.1100000003</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1895,15 +1836,15 @@
     <row r="9" spans="1:4">
       <c r="B9" s="3">
         <f>SUM(B2:B8)</f>
-        <v>129.41</v>
+        <v>141.74</v>
       </c>
       <c r="C9" s="3">
         <f>SUM(C2:C8)</f>
-        <v>8460.2199999999993</v>
+        <v>11498.94</v>
       </c>
       <c r="D9" s="3">
         <f>SUM(D2:D8)</f>
-        <v>235676432.63</v>
+        <v>237918977.63</v>
       </c>
     </row>
     <row r="10" spans="1:4">

</xml_diff>

<commit_message>
Adding Costs-Graphics and adding Architektur
</commit_message>
<xml_diff>
--- a/dokumentation/costs-aws-virtualdesktop.xlsx
+++ b/dokumentation/costs-aws-virtualdesktop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Dropbox\Studium\Master\IV Semester\CloudComputing\VirtualDesktop-Master\dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3531F940-C245-453E-A1F6-7C29DF48EF11}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339F8AAB-2A1F-4C52-B488-FAE881F93E3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204" xr2:uid="{6BB69F5D-5E78-4C76-8896-0945FFA67CA2}"/>
   </bookViews>
@@ -180,9 +180,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="percentStacked"/>
+      <c:areaChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -207,45 +206,38 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$B$1:$D$1</c:f>
+              <c:f>Tabelle1!$B$1:$C$1</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>10 pro Minute</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1000 pro Minute</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000000 pro Minute</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$2:$D$2</c:f>
+              <c:f>Tabelle1!$B$2:$C$2</c:f>
               <c:numCache>
                 <c:formatCode>[$$-409]#,##0.00</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>4.18</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>8.86</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>52003.66</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-74A0-4B3B-A85B-3327C8E793C9}"/>
+              <c16:uniqueId val="{00000000-F3E5-44D5-8100-2FB501111BC1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -272,45 +264,38 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$B$1:$D$1</c:f>
+              <c:f>Tabelle1!$B$1:$C$1</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>10 pro Minute</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1000 pro Minute</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000000 pro Minute</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$3:$D$3</c:f>
+              <c:f>Tabelle1!$B$3:$C$3</c:f>
               <c:numCache>
                 <c:formatCode>[$$-409]#,##0.00</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>3.34</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>344.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>230416764.75999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-74A0-4B3B-A85B-3327C8E793C9}"/>
+              <c16:uniqueId val="{00000001-F3E5-44D5-8100-2FB501111BC1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -332,50 +317,43 @@
             <a:solidFill>
               <a:schemeClr val="accent3"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="25400">
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$B$1:$D$1</c:f>
+              <c:f>Tabelle1!$B$1:$C$1</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>10 pro Minute</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1000 pro Minute</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000000 pro Minute</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$4:$D$4</c:f>
+              <c:f>Tabelle1!$B$4:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>[$$-409]#,##0.00</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>17.7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8960.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-74A0-4B3B-A85B-3327C8E793C9}"/>
+              <c16:uniqueId val="{00000002-F3E5-44D5-8100-2FB501111BC1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -397,50 +375,43 @@
             <a:solidFill>
               <a:schemeClr val="accent4"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="25400">
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$B$1:$D$1</c:f>
+              <c:f>Tabelle1!$B$1:$C$1</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>10 pro Minute</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1000 pro Minute</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000000 pro Minute</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$5:$D$5</c:f>
+              <c:f>Tabelle1!$B$5:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>[$$-409]#,##0.00</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.31</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-74A0-4B3B-A85B-3327C8E793C9}"/>
+              <c16:uniqueId val="{00000003-F3E5-44D5-8100-2FB501111BC1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -462,42 +433,35 @@
             <a:solidFill>
               <a:schemeClr val="accent5"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="25400">
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$B$1:$D$1</c:f>
+              <c:f>Tabelle1!$B$1:$C$1</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>10 pro Minute</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1000 pro Minute</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000000 pro Minute</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$6:$D$6</c:f>
+              <c:f>Tabelle1!$B$6:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>[$$-409]#,##0.00</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -505,7 +469,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-74A0-4B3B-A85B-3327C8E793C9}"/>
+              <c16:uniqueId val="{00000004-F3E5-44D5-8100-2FB501111BC1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -527,50 +491,43 @@
             <a:solidFill>
               <a:schemeClr val="accent6"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="25400">
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$B$1:$D$1</c:f>
+              <c:f>Tabelle1!$B$1:$C$1</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>10 pro Minute</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1000 pro Minute</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000000 pro Minute</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$7:$D$7</c:f>
+              <c:f>Tabelle1!$B$7:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>[$$-409]#,##0.00</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>131.49</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>11053.11</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7366451.1100000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-74A0-4B3B-A85B-3327C8E793C9}"/>
+              <c16:uniqueId val="{00000005-F3E5-44D5-8100-2FB501111BC1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -594,50 +551,43 @@
                 <a:lumMod val="60000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="25400">
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$B$1:$D$1</c:f>
+              <c:f>Tabelle1!$B$1:$C$1</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>10 pro Minute</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1000 pro Minute</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000000 pro Minute</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$8:$D$8</c:f>
+              <c:f>Tabelle1!$B$8:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>[$$-409]#,##0.00</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>2.0299999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>74.760000000000005</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>74766.600000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-74A0-4B3B-A85B-3327C8E793C9}"/>
+              <c16:uniqueId val="{00000006-F3E5-44D5-8100-2FB501111BC1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -649,19 +599,82 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:overlap val="100"/>
-        <c:axId val="443142704"/>
-        <c:axId val="443143688"/>
-      </c:barChart>
+        <c:axId val="496439664"/>
+        <c:axId val="547368848"/>
+      </c:areaChart>
       <c:catAx>
-        <c:axId val="443142704"/>
+        <c:axId val="496439664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="547368848"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="547368848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="[$$-409]#,##0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -692,68 +705,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443143688"/>
+        <c:crossAx val="496439664"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="443143688"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="443142704"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -795,14 +749,7 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
+    <c:dispBlanksAs val="zero"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -879,7 +826,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="276">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -902,6 +849,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
@@ -1138,20 +1096,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
@@ -1162,6 +1106,25 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
   </cs:gridlineMajor>
   <cs:gridlineMinor>
     <cs:lnRef idx="0"/>
@@ -1258,6 +1221,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1376,23 +1350,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>350520</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>373380</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Diagramm 1">
+        <xdr:cNvPr id="3" name="Diagramm 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F957D65-E929-41BD-AAE0-98CE6074DFD1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3647397A-248E-4870-8057-4685755503B0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1713,7 +1687,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C8" sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Extending Doku fixing template
</commit_message>
<xml_diff>
--- a/dokumentation/costs-aws-virtualdesktop.xlsx
+++ b/dokumentation/costs-aws-virtualdesktop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Dropbox\Studium\Master\IV Semester\CloudComputing\VirtualDesktop-Master\dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339F8AAB-2A1F-4C52-B488-FAE881F93E3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850E1CFD-78C7-403B-8489-22226B5E156A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204" xr2:uid="{6BB69F5D-5E78-4C76-8896-0945FFA67CA2}"/>
   </bookViews>
@@ -30,16 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>10 pro Minute</t>
-  </si>
-  <si>
-    <t>1000 pro Minute</t>
-  </si>
-  <si>
-    <t>1000000 pro Minute</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>EC2</t>
   </si>
@@ -60,6 +51,18 @@
   </si>
   <si>
     <t>Lambda</t>
+  </si>
+  <si>
+    <t>1000000 Nutzer</t>
+  </si>
+  <si>
+    <t>1000 Nutzer</t>
+  </si>
+  <si>
+    <t>10 Nutzer</t>
+  </si>
+  <si>
+    <t>Cognito</t>
   </si>
 </sst>
 </file>
@@ -178,10 +181,50 @@
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
     <c:plotArea>
       <c:layout/>
-      <c:areaChart>
-        <c:grouping val="standard"/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -205,39 +248,47 @@
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
+            <a:sp3d/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$B$1:$C$1</c:f>
+              <c:f>Tabelle1!$B$1:$D$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>10 pro Minute</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10 Nutzer</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1000 pro Minute</c:v>
+                  <c:v>1000 Nutzer</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000000 Nutzer</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$2:$C$2</c:f>
+              <c:f>Tabelle1!$B$2:$D$2</c:f>
               <c:numCache>
                 <c:formatCode>[$$-409]#,##0.00</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>4.18</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>8.86</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5203.66</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F3E5-44D5-8100-2FB501111BC1}"/>
+              <c16:uniqueId val="{00000000-2415-42B4-BC83-62CB21ACB418}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -263,39 +314,47 @@
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
+            <a:sp3d/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$B$1:$C$1</c:f>
+              <c:f>Tabelle1!$B$1:$D$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>10 pro Minute</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10 Nutzer</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1000 pro Minute</c:v>
+                  <c:v>1000 Nutzer</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000000 Nutzer</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$3:$C$3</c:f>
+              <c:f>Tabelle1!$B$3:$D$3</c:f>
               <c:numCache>
                 <c:formatCode>[$$-409]#,##0.00</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>3.34</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.14000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>344.2</c:v>
+                  <c:v>11.06</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9936.76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F3E5-44D5-8100-2FB501111BC1}"/>
+              <c16:uniqueId val="{00000001-2415-42B4-BC83-62CB21ACB418}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -317,43 +376,51 @@
             <a:solidFill>
               <a:schemeClr val="accent3"/>
             </a:solidFill>
-            <a:ln w="25400">
+            <a:ln>
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
+            <a:sp3d/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$B$1:$C$1</c:f>
+              <c:f>Tabelle1!$B$1:$D$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>10 pro Minute</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10 Nutzer</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1000 pro Minute</c:v>
+                  <c:v>1000 Nutzer</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000000 Nutzer</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$4:$C$4</c:f>
+              <c:f>Tabelle1!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>[$$-409]#,##0.00</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.7</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.7</c:v>
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>882.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-F3E5-44D5-8100-2FB501111BC1}"/>
+              <c16:uniqueId val="{00000002-2415-42B4-BC83-62CB21ACB418}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -375,43 +442,51 @@
             <a:solidFill>
               <a:schemeClr val="accent4"/>
             </a:solidFill>
-            <a:ln w="25400">
+            <a:ln>
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
+            <a:sp3d/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$B$1:$C$1</c:f>
+              <c:f>Tabelle1!$B$1:$D$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>10 pro Minute</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10 Nutzer</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1000 pro Minute</c:v>
+                  <c:v>1000 Nutzer</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000000 Nutzer</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$5:$C$5</c:f>
+              <c:f>Tabelle1!$B$5:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>[$$-409]#,##0.00</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.31</c:v>
+                  <c:v>3.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13349.48</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-F3E5-44D5-8100-2FB501111BC1}"/>
+              <c16:uniqueId val="{00000003-2415-42B4-BC83-62CB21ACB418}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -433,35 +508,43 @@
             <a:solidFill>
               <a:schemeClr val="accent5"/>
             </a:solidFill>
-            <a:ln w="25400">
+            <a:ln>
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
+            <a:sp3d/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$B$1:$C$1</c:f>
+              <c:f>Tabelle1!$B$1:$D$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>10 pro Minute</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10 Nutzer</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1000 pro Minute</c:v>
+                  <c:v>1000 Nutzer</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000000 Nutzer</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$6:$C$6</c:f>
+              <c:f>Tabelle1!$B$6:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>[$$-409]#,##0.00</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -469,7 +552,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-F3E5-44D5-8100-2FB501111BC1}"/>
+              <c16:uniqueId val="{00000004-2415-42B4-BC83-62CB21ACB418}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -491,43 +574,51 @@
             <a:solidFill>
               <a:schemeClr val="accent6"/>
             </a:solidFill>
-            <a:ln w="25400">
+            <a:ln>
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
+            <a:sp3d/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$B$1:$C$1</c:f>
+              <c:f>Tabelle1!$B$1:$D$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>10 pro Minute</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10 Nutzer</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1000 pro Minute</c:v>
+                  <c:v>1000 Nutzer</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000000 Nutzer</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$7:$C$7</c:f>
+              <c:f>Tabelle1!$B$7:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>[$$-409]#,##0.00</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>131.49</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>9.6300000000000008</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11053.11</c:v>
+                  <c:v>969.11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>543891.11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-F3E5-44D5-8100-2FB501111BC1}"/>
+              <c16:uniqueId val="{00000005-2415-42B4-BC83-62CB21ACB418}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -540,7 +631,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Lambda</c:v>
+                  <c:v>Cognito</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -551,43 +642,119 @@
                 <a:lumMod val="60000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:ln w="25400">
+            <a:ln>
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
+            <a:sp3d/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$B$1:$C$1</c:f>
+              <c:f>Tabelle1!$B$1:$D$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>10 pro Minute</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10 Nutzer</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1000 pro Minute</c:v>
+                  <c:v>1000 Nutzer</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000000 Nutzer</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$8:$C$8</c:f>
+              <c:f>Tabelle1!$B$8:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>[$$-409]#,##0.00</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>2.0299999999999998</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>74.760000000000005</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4415</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-F3E5-44D5-8100-2FB501111BC1}"/>
+              <c16:uniqueId val="{00000006-2415-42B4-BC83-62CB21ACB418}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lambda</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tabelle1!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10 Nutzer</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000 Nutzer</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000000 Nutzer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$9:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>[$$-409]#,##0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.3999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.3899999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4392</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-2415-42B4-BC83-62CB21ACB418}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -599,30 +766,27 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="496439664"/>
-        <c:axId val="547368848"/>
-      </c:areaChart>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="560909344"/>
+        <c:axId val="560902784"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
       <c:catAx>
-        <c:axId val="496439664"/>
+        <c:axId val="560909344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -646,7 +810,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="547368848"/>
+        <c:crossAx val="560902784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -654,7 +818,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="547368848"/>
+        <c:axId val="560902784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -705,9 +869,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="496439664"/>
+        <c:crossAx val="560909344"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -749,7 +913,14 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -826,7 +997,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="276">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -849,17 +1020,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
@@ -1096,14 +1256,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
       </a:ln>
     </cs:spPr>
   </cs:floor>
@@ -1221,17 +1376,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1350,23 +1494,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>121920</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Diagramm 2">
+        <xdr:cNvPr id="2" name="Diagramm 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3647397A-248E-4870-8057-4685755503B0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C226E2C8-8550-444E-BC79-64347766AAD9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1687,7 +1831,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="A1:C8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1700,18 +1844,18 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>4.18</v>
@@ -1720,54 +1864,54 @@
         <v>8.86</v>
       </c>
       <c r="D2" s="2">
-        <v>52003.66</v>
+        <v>5203.66</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>3.34</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="C3" s="2">
-        <v>344.2</v>
+        <v>11.06</v>
       </c>
       <c r="D3" s="2">
-        <v>230416764.75999999</v>
+        <v>9936.76</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="C4" s="2">
-        <v>17.7</v>
+        <v>2.1</v>
       </c>
       <c r="D4" s="2">
-        <v>8960.5</v>
+        <v>882.5</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>0</v>
+        <v>0.31</v>
       </c>
       <c r="C5" s="2">
-        <v>0.31</v>
+        <v>3.05</v>
       </c>
       <c r="D5" s="2">
-        <v>31</v>
+        <v>13349.48</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -1781,48 +1925,59 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>131.49</v>
+        <v>9.6300000000000008</v>
       </c>
       <c r="C7" s="2">
-        <v>11053.11</v>
+        <v>969.11</v>
       </c>
       <c r="D7" s="2">
-        <v>7366451.1100000003</v>
+        <v>543891.11</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
+      <c r="A8" t="s">
+        <v>10</v>
       </c>
       <c r="B8" s="2">
-        <v>2.0299999999999998</v>
+        <v>0</v>
       </c>
       <c r="C8" s="2">
-        <v>74.760000000000005</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2">
-        <v>74766.600000000006</v>
+        <v>4415</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="B9" s="3">
-        <f>SUM(B2:B8)</f>
-        <v>141.74</v>
-      </c>
-      <c r="C9" s="3">
-        <f>SUM(C2:C8)</f>
-        <v>11498.94</v>
-      </c>
-      <c r="D9" s="3">
-        <f>SUM(D2:D8)</f>
-        <v>237918977.63</v>
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="C9" s="2">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="D9" s="2">
+        <v>4392</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="B10"/>
+      <c r="B10" s="3">
+        <f>SUM(B2:B9)</f>
+        <v>15.204000000000001</v>
+      </c>
+      <c r="C10" s="3">
+        <f>SUM(C2:C9)</f>
+        <v>998.57</v>
+      </c>
+      <c r="D10" s="3">
+        <f>SUM(D2:D9)</f>
+        <v>582070.51</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="B11"/>

</xml_diff>